<commit_message>
final V commit w color back
</commit_message>
<xml_diff>
--- a/Basic-Py-Projects/basic_CRUD_in_py/data/UX_guide.xlsx
+++ b/Basic-Py-Projects/basic_CRUD_in_py/data/UX_guide.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lfcct\Desktop\progams\basic_CRUD_in_py\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lfcct\Desktop\progams\basic_CRUD_in_py\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641BAD18-5B10-4F7A-AFE9-272E288F182E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8D7D7B-DFE4-4C5B-9971-99950A753674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="1110" windowWidth="14685" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>ux_id</t>
   </si>
@@ -37,6 +37,21 @@
   </si>
   <si>
     <t>...</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>green</t>
   </si>
 </sst>
 </file>
@@ -93,8 +108,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E3A464CE-9BBA-40A1-A30C-43BBBEC5FA13}" name="Tabela1" displayName="Tabela1" ref="A1:C2" totalsRowShown="0">
-  <autoFilter ref="A1:C2" xr:uid="{E3A464CE-9BBA-40A1-A30C-43BBBEC5FA13}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E3A464CE-9BBA-40A1-A30C-43BBBEC5FA13}" name="Tabela1" displayName="Tabela1" ref="A1:C6" totalsRowShown="0">
+  <autoFilter ref="A1:C6" xr:uid="{E3A464CE-9BBA-40A1-A30C-43BBBEC5FA13}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0448D629-639A-4DA8-80AB-FFFCFC37685D}" name="ux_id"/>
     <tableColumn id="2" xr3:uid="{5F35A68C-6DEF-4D8A-B409-1AE8A75257C8}" name="info"/>
@@ -370,7 +385,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,7 +409,39 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>